<commit_message>
Make table for tutorials
</commit_message>
<xml_diff>
--- a/tutorials/code_gallery.csv.xlsx
+++ b/tutorials/code_gallery.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madisonrichardson/CoastWatch-Training-Tutorials/tutorials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B008A75-495D-0F4E-97FD-CF66E6C62DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4919725-812E-5041-9D64-28427F8BEFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{0A27945C-3EF8-BC47-BA08-A8FF32C0CF2F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>title</t>
   </si>
@@ -89,6 +89,45 @@
   </si>
   <si>
     <t>tutorials/time-series/compare-sensors.Rmd</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>previews</t>
+  </si>
+  <si>
+    <t>Description here.</t>
+  </si>
+  <si>
+    <t>previews/lon_180_to_360/p1.png</t>
+  </si>
+  <si>
+    <t>previews/compare_sensors/p1.png</t>
+  </si>
+  <si>
+    <t>modal_id</t>
+  </si>
+  <si>
+    <t>modal-lon</t>
+  </si>
+  <si>
+    <t>modal-chla</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Description here</t>
+  </si>
+  <si>
+    <t>preview_image</t>
+  </si>
+  <si>
+    <t>previews/lon.png</t>
+  </si>
+  <si>
+    <t>previews/chla.png</t>
   </si>
 </sst>
 </file>
@@ -446,23 +485,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E148623C-B8A9-F64D-A993-4856F245370B}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,25 +510,40 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -496,30 +551,60 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>